<commit_message>
Action map and EER update
</commit_message>
<xml_diff>
--- a/ActionMapAndEER/ActionMap.xlsx
+++ b/ActionMapAndEER/ActionMap.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88375448-F808-4106-B35C-54508098B5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F21ADB-BD79-4959-8B90-03D1A5D7AF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$4:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$4:$F$35</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -233,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -287,13 +287,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -311,7 +311,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -320,52 +320,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -380,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,34 +343,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,25 +646,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="B3:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28.44140625" customWidth="1"/>
-    <col min="3" max="8" width="28.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="1" customWidth="1"/>
+    <col min="4" max="8" width="28.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -736,48 +677,44 @@
       <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
+      <c r="G4"/>
+      <c r="H4"/>
     </row>
     <row r="5" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5"/>
+      <c r="H5"/>
     </row>
     <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6"/>
+      <c r="H6"/>
     </row>
     <row r="7" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="12"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7"/>
+      <c r="H7"/>
     </row>
     <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -790,50 +727,52 @@
         <v>13</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3"/>
+      <c r="G8"/>
+      <c r="H8"/>
     </row>
     <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9"/>
+      <c r="H9"/>
     </row>
     <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="F10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
     </row>
     <row r="11" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11"/>
+      <c r="H11"/>
     </row>
     <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -844,48 +783,48 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
+      <c r="G12"/>
+      <c r="H12"/>
     </row>
     <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13"/>
+      <c r="H13"/>
     </row>
     <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14"/>
+      <c r="H14"/>
     </row>
     <row r="15" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15"/>
+      <c r="H15"/>
     </row>
     <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -894,44 +833,42 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
+      <c r="G16"/>
+      <c r="H16"/>
     </row>
     <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17"/>
+      <c r="H17"/>
     </row>
     <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
-      <c r="C18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18"/>
+      <c r="H18"/>
     </row>
     <row r="19" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="12"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="10" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19"/>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -940,38 +877,38 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="11"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="12"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
+      <c r="G20"/>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="7"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="2:8" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="8"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23"/>
+      <c r="H23"/>
     </row>
     <row r="24" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -980,40 +917,40 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="3"/>
+      <c r="G24"/>
+      <c r="H24"/>
     </row>
     <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="11"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="5"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25"/>
+      <c r="H25"/>
     </row>
     <row r="26" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26"/>
+      <c r="H26"/>
     </row>
     <row r="27" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="12"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27"/>
+      <c r="H27"/>
     </row>
     <row r="28" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1022,42 +959,42 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="3"/>
+      <c r="G28"/>
+      <c r="H28"/>
     </row>
     <row r="29" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="11"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="5"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29"/>
+      <c r="H29"/>
     </row>
     <row r="30" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B30" s="11"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30"/>
+      <c r="H30"/>
     </row>
     <row r="31" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="12"/>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31"/>
+      <c r="H31"/>
     </row>
     <row r="32" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1068,52 +1005,56 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="3"/>
+      <c r="G32"/>
+      <c r="H32"/>
     </row>
     <row r="33" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B33" s="11"/>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="5"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33"/>
+      <c r="H33"/>
     </row>
     <row r="34" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="11"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34"/>
+      <c r="H34"/>
     </row>
     <row r="35" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="12"/>
-      <c r="C35" s="8" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="9"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35"/>
+      <c r="H35"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B15"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.51" right="0.25" top="2.09" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="150" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Categories add and edit, and pojos switched from data to getter and setters
</commit_message>
<xml_diff>
--- a/ActionMapAndEER/ActionMap.xlsx
+++ b/ActionMapAndEER/ActionMap.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F21ADB-BD79-4959-8B90-03D1A5D7AF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AD96AC-9E69-43F0-B766-A71B8C59A05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$4:$F$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$4:$F$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>register</t>
   </si>
@@ -97,24 +97,15 @@
     <t>addCategory</t>
   </si>
   <si>
-    <t>addDiscountForCategory</t>
-  </si>
-  <si>
     <t>editCategory</t>
   </si>
   <si>
     <t>getAllCategories</t>
   </si>
   <si>
-    <t>getProductsFromCategory</t>
-  </si>
-  <si>
     <t>deleteCategory</t>
   </si>
   <si>
-    <t>removeDiscountForCategory</t>
-  </si>
-  <si>
     <t>cart</t>
   </si>
   <si>
@@ -164,6 +155,21 @@
   </si>
   <si>
     <t>deleteReview</t>
+  </si>
+  <si>
+    <t>getSubcategoriesFromCategory</t>
+  </si>
+  <si>
+    <t>sub_categories</t>
+  </si>
+  <si>
+    <t>addSubcategory</t>
+  </si>
+  <si>
+    <t>editSubcategory</t>
+  </si>
+  <si>
+    <t>deleteSubcategory</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -331,11 +337,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,6 +402,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,17 +698,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H35"/>
+  <dimension ref="B3:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="61" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H22:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="1" customWidth="1"/>
-    <col min="4" max="8" width="28.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" style="1" customWidth="1"/>
+    <col min="5" max="8" width="28.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -771,25 +824,23 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>22</v>
+    <row r="12" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
+    <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -797,38 +848,34 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+    <row r="14" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
       <c r="C14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="8"/>
+    <row r="15" spans="2:8" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="11"/>
       <c r="C15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>30</v>
+    <row r="16" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -836,10 +883,10 @@
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
+    <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10"/>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -847,19 +894,21 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="4"/>
+    <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10"/>
+      <c r="C18" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="8"/>
+    <row r="19" spans="2:8" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="11"/>
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -867,12 +916,12 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -880,16 +929,18 @@
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -898,21 +949,23 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="2:8" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="8"/>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -920,7 +973,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -929,18 +982,16 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -951,10 +1002,10 @@
     </row>
     <row r="28" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -974,7 +1025,7 @@
     <row r="30" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="4" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -984,9 +1035,7 @@
     </row>
     <row r="31" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="8"/>
-      <c r="C31" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -995,14 +1044,12 @@
     </row>
     <row r="32" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32"/>
@@ -1010,9 +1057,7 @@
     </row>
     <row r="33" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
-      <c r="C33" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1022,11 +1067,9 @@
     <row r="34" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34"/>
@@ -1035,7 +1078,7 @@
     <row r="35" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8"/>
       <c r="C35" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -1043,18 +1086,69 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
+    <row r="36" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="7"/>
+      <c r="C37" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="7"/>
+      <c r="C38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="8"/>
+      <c r="C39" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39"/>
+      <c r="H39"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B32:B35"/>
+  <mergeCells count="9">
+    <mergeCell ref="B36:B39"/>
     <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.51" right="0.25" top="2.09" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="150" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="121" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Product addProduct() --- needs fix
</commit_message>
<xml_diff>
--- a/ActionMapAndEER/ActionMap.xlsx
+++ b/ActionMapAndEER/ActionMap.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F21ADB-BD79-4959-8B90-03D1A5D7AF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AD96AC-9E69-43F0-B766-A71B8C59A05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$4:$F$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$4:$F$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>register</t>
   </si>
@@ -97,24 +97,15 @@
     <t>addCategory</t>
   </si>
   <si>
-    <t>addDiscountForCategory</t>
-  </si>
-  <si>
     <t>editCategory</t>
   </si>
   <si>
     <t>getAllCategories</t>
   </si>
   <si>
-    <t>getProductsFromCategory</t>
-  </si>
-  <si>
     <t>deleteCategory</t>
   </si>
   <si>
-    <t>removeDiscountForCategory</t>
-  </si>
-  <si>
     <t>cart</t>
   </si>
   <si>
@@ -164,6 +155,21 @@
   </si>
   <si>
     <t>deleteReview</t>
+  </si>
+  <si>
+    <t>getSubcategoriesFromCategory</t>
+  </si>
+  <si>
+    <t>sub_categories</t>
+  </si>
+  <si>
+    <t>addSubcategory</t>
+  </si>
+  <si>
+    <t>editSubcategory</t>
+  </si>
+  <si>
+    <t>deleteSubcategory</t>
   </si>
 </sst>
 </file>
@@ -233,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -331,11 +337,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,6 +402,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,17 +698,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:H35"/>
+  <dimension ref="B3:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="61" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H22:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="1" customWidth="1"/>
-    <col min="4" max="8" width="28.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" style="1" customWidth="1"/>
+    <col min="5" max="8" width="28.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -771,25 +824,23 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>22</v>
+    <row r="12" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
+    <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -797,38 +848,34 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+    <row r="14" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
       <c r="C14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="8"/>
+    <row r="15" spans="2:8" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="11"/>
       <c r="C15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>30</v>
+    <row r="16" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -836,10 +883,10 @@
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
+    <row r="17" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10"/>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -847,19 +894,21 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="4"/>
+    <row r="18" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10"/>
+      <c r="C18" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="8"/>
+    <row r="19" spans="2:8" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="11"/>
       <c r="C19" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -867,12 +916,12 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -880,16 +929,18 @@
       <c r="G20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -898,21 +949,23 @@
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="2:8" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="8"/>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -920,7 +973,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -929,18 +982,16 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -951,10 +1002,10 @@
     </row>
     <row r="28" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -974,7 +1025,7 @@
     <row r="30" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="7"/>
       <c r="C30" s="4" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -984,9 +1035,7 @@
     </row>
     <row r="31" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="8"/>
-      <c r="C31" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -995,14 +1044,12 @@
     </row>
     <row r="32" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32"/>
@@ -1010,9 +1057,7 @@
     </row>
     <row r="33" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
-      <c r="C33" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1022,11 +1067,9 @@
     <row r="34" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34"/>
@@ -1035,7 +1078,7 @@
     <row r="35" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8"/>
       <c r="C35" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -1043,18 +1086,69 @@
       <c r="G35"/>
       <c r="H35"/>
     </row>
+    <row r="36" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="7"/>
+      <c r="C37" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="7"/>
+      <c r="C38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="8"/>
+      <c r="C39" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39"/>
+      <c r="H39"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B32:B35"/>
+  <mergeCells count="9">
+    <mergeCell ref="B36:B39"/>
     <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.51" right="0.25" top="2.09" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="150" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="121" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added subcategories and discounts logic
</commit_message>
<xml_diff>
--- a/ActionMapAndEER/ActionMap.xlsx
+++ b/ActionMapAndEER/ActionMap.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AD96AC-9E69-43F0-B766-A71B8C59A05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB8BE0A-62DE-46C6-B29B-34EB029942DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>register</t>
   </si>
@@ -121,12 +121,6 @@
     <t>orders</t>
   </si>
   <si>
-    <t>coupons</t>
-  </si>
-  <si>
-    <t>addCoupon</t>
-  </si>
-  <si>
     <t>createOrder</t>
   </si>
   <si>
@@ -170,6 +164,12 @@
   </si>
   <si>
     <t>deleteSubcategory</t>
+  </si>
+  <si>
+    <t>discounts</t>
+  </si>
+  <si>
+    <t>addDiscount</t>
   </si>
 </sst>
 </file>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="61" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H22:I23"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,10 +826,10 @@
     </row>
     <row r="12" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -840,7 +840,7 @@
     <row r="13" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10"/>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -851,7 +851,7 @@
     <row r="14" spans="2:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
       <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -862,7 +862,7 @@
     <row r="15" spans="2:8" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
       <c r="C15" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -942,7 +942,9 @@
     </row>
     <row r="22" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -960,12 +962,12 @@
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -973,7 +975,7 @@
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -982,7 +984,7 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="2:8" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -991,7 +993,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="2:8" ht="16.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1005,7 +1007,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1044,10 +1046,10 @@
     </row>
     <row r="32" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1067,7 +1069,7 @@
     <row r="34" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1078,7 +1080,7 @@
     <row r="35" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8"/>
       <c r="C35" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -1088,13 +1090,13 @@
     </row>
     <row r="36" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1104,7 +1106,7 @@
     <row r="37" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
       <c r="C37" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -1128,7 +1130,7 @@
     <row r="39" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="8"/>
       <c r="C39" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -1149,6 +1151,6 @@
     <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.51" right="0.25" top="2.09" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="121" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="108" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Product -> getFav , serchByKeyword
</commit_message>
<xml_diff>
--- a/ActionMapAndEER/ActionMap.xlsx
+++ b/ActionMapAndEER/ActionMap.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B44A99F-CA09-4B3F-9636-F2D661FE6BFA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C662335-C510-4CF6-9447-8FEEC3B0C874}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,53 +431,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -485,6 +485,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -774,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C4:C19"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -792,122 +795,122 @@
   <sheetData>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="H4"/>
       <c r="I4"/>
     </row>
     <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
       <c r="H5"/>
       <c r="I5"/>
     </row>
     <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
       <c r="H6"/>
       <c r="I6"/>
     </row>
     <row r="7" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
       <c r="H7"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
       <c r="H8"/>
       <c r="I8"/>
     </row>
     <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
       <c r="H9"/>
       <c r="I9"/>
     </row>
     <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
     </row>
     <row r="11" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
       <c r="H11"/>
       <c r="I11"/>
     </row>
@@ -915,49 +918,49 @@
       <c r="B12" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
       <c r="H12"/>
       <c r="I12"/>
     </row>
     <row r="13" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="17"/>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
       <c r="H13"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="17"/>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
       <c r="H14"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="2:9" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
       <c r="H15"/>
       <c r="I15"/>
     </row>
@@ -965,291 +968,291 @@
       <c r="B16" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
       <c r="H16"/>
       <c r="I16"/>
     </row>
     <row r="17" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="17"/>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
       <c r="H17"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17"/>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="11"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
       <c r="H18"/>
       <c r="I18"/>
     </row>
     <row r="19" spans="2:9" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="18"/>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
       <c r="H19"/>
       <c r="I19"/>
     </row>
     <row r="20" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
       <c r="H20"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
       <c r="H21"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
       <c r="H22"/>
       <c r="I22"/>
     </row>
     <row r="23" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="12"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="15"/>
+      <c r="C23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
       <c r="H23"/>
       <c r="I23"/>
     </row>
     <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
       <c r="H24"/>
       <c r="I24"/>
     </row>
     <row r="25" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
       <c r="H25"/>
       <c r="I25"/>
     </row>
     <row r="26" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
       <c r="H26"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
       <c r="H27"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="4"/>
       <c r="H28"/>
       <c r="I28"/>
     </row>
     <row r="29" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B29" s="6"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="9"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="7"/>
       <c r="H29"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B30" s="6"/>
-      <c r="C30" s="10" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
       <c r="H30"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
       <c r="H31"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="5"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="4"/>
       <c r="H32"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B33" s="6"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
       <c r="H33"/>
       <c r="I33"/>
     </row>
     <row r="34" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B34" s="6"/>
-      <c r="C34" s="10" t="s">
+      <c r="B34" s="14"/>
+      <c r="C34" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="11"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
       <c r="H34"/>
       <c r="I34"/>
     </row>
     <row r="35" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="12"/>
-      <c r="C35" s="13" t="s">
+      <c r="B35" s="15"/>
+      <c r="C35" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="14"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
       <c r="H35"/>
       <c r="I35"/>
     </row>
     <row r="36" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="5"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="4"/>
       <c r="H36"/>
       <c r="I36"/>
     </row>
     <row r="37" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B37" s="6"/>
-      <c r="C37" s="8" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="9"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="7"/>
       <c r="H37"/>
       <c r="I37"/>
     </row>
     <row r="38" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B38" s="6"/>
-      <c r="C38" s="10" t="s">
+      <c r="B38" s="14"/>
+      <c r="C38" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="11"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="9"/>
       <c r="H38"/>
       <c r="I38"/>
     </row>
     <row r="39" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="12"/>
-      <c r="C39" s="13" t="s">
+      <c r="B39" s="15"/>
+      <c r="C39" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="14"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="11"/>
       <c r="H39"/>
       <c r="I39"/>
     </row>
@@ -1265,7 +1268,7 @@
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="B12:B15"/>
   </mergeCells>
-  <pageMargins left="0.51" right="0.25" top="2.09" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="89" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.25" top="0.94" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cart and many other
</commit_message>
<xml_diff>
--- a/ActionMapAndEER/ActionMap.xlsx
+++ b/ActionMapAndEER/ActionMap.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C662335-C510-4CF6-9447-8FEEC3B0C874}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D97AA35-A4AC-4667-890F-A5E47CB52989}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>register</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>addDiscountToProduct</t>
+  </si>
+  <si>
+    <t>subscribe</t>
+  </si>
+  <si>
+    <t>unsubscribe</t>
+  </si>
+  <si>
+    <t>getProductsBySubcategorySortedBy</t>
   </si>
 </sst>
 </file>
@@ -469,6 +478,9 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -485,9 +497,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -778,7 +787,7 @@
   <dimension ref="B3:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C23"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,22 +795,22 @@
     <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="28.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="35.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -811,23 +820,27 @@
         <v>3</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4"/>
+      <c r="H4" s="4"/>
       <c r="I4"/>
     </row>
     <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
-      <c r="H5"/>
+      <c r="H5" s="7"/>
       <c r="I5"/>
     </row>
     <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
@@ -837,21 +850,21 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
-      <c r="H6"/>
+      <c r="H6" s="9"/>
       <c r="I6"/>
     </row>
     <row r="7" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="15"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
-      <c r="H7"/>
+      <c r="H7" s="11"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -865,11 +878,11 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
-      <c r="H8"/>
+      <c r="H8" s="4"/>
       <c r="I8"/>
     </row>
     <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
@@ -877,11 +890,11 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
-      <c r="H9"/>
+      <c r="H9" s="7"/>
       <c r="I9"/>
     </row>
     <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
@@ -891,17 +904,16 @@
       <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="19" t="s">
+      <c r="F10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H10"/>
+      <c r="G10" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="12" t="s">
         <v>18</v>
       </c>
@@ -911,11 +923,11 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
-      <c r="H11"/>
+      <c r="H11" s="11"/>
       <c r="I11"/>
     </row>
     <row r="12" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -925,11 +937,11 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
-      <c r="H12"/>
+      <c r="H12" s="4"/>
       <c r="I12"/>
     </row>
     <row r="13" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="5" t="s">
         <v>45</v>
       </c>
@@ -937,11 +949,11 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
-      <c r="H13"/>
+      <c r="H13" s="7"/>
       <c r="I13"/>
     </row>
     <row r="14" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5" t="s">
         <v>42</v>
       </c>
@@ -949,11 +961,11 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
-      <c r="H14"/>
+      <c r="H14" s="9"/>
       <c r="I14"/>
     </row>
     <row r="15" spans="2:9" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="18"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="12" t="s">
         <v>46</v>
       </c>
@@ -961,11 +973,11 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
-      <c r="H15"/>
+      <c r="H15" s="11"/>
       <c r="I15"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -975,11 +987,11 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
-      <c r="H16"/>
+      <c r="H16" s="4"/>
       <c r="I16"/>
     </row>
     <row r="17" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="5" t="s">
         <v>24</v>
       </c>
@@ -987,11 +999,11 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7"/>
-      <c r="H17"/>
+      <c r="H17" s="7"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
@@ -999,11 +1011,11 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
-      <c r="H18"/>
+      <c r="H18" s="9"/>
       <c r="I18"/>
     </row>
     <row r="19" spans="2:9" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="18"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
@@ -1011,25 +1023,25 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
-      <c r="H19"/>
+      <c r="H19" s="11"/>
       <c r="I19"/>
     </row>
     <row r="20" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
-      <c r="H20"/>
+      <c r="H20" s="4"/>
       <c r="I20"/>
     </row>
     <row r="21" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B21" s="14"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="6" t="s">
         <v>29</v>
       </c>
@@ -1037,35 +1049,35 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7"/>
-      <c r="H21"/>
+      <c r="H21" s="7"/>
       <c r="I21"/>
     </row>
     <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B22" s="14"/>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="15"/>
+      <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="9"/>
-      <c r="H22"/>
+      <c r="H22" s="9"/>
       <c r="I22"/>
     </row>
     <row r="23" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
-      <c r="H23"/>
+      <c r="H23" s="11"/>
       <c r="I23"/>
     </row>
     <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1075,41 +1087,41 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
-      <c r="H24"/>
+      <c r="H24" s="4"/>
       <c r="I24"/>
     </row>
     <row r="25" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B25" s="14"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="7"/>
-      <c r="H25"/>
+      <c r="H25" s="7"/>
       <c r="I25"/>
     </row>
     <row r="26" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B26" s="14"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
-      <c r="H26"/>
+      <c r="H26" s="9"/>
       <c r="I26"/>
     </row>
     <row r="27" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="15"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="11"/>
-      <c r="H27"/>
+      <c r="H27" s="11"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1119,21 +1131,21 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="4"/>
-      <c r="H28"/>
+      <c r="H28" s="4"/>
       <c r="I28"/>
     </row>
     <row r="29" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B29" s="14"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7"/>
-      <c r="H29"/>
+      <c r="H29" s="7"/>
       <c r="I29"/>
     </row>
     <row r="30" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B30" s="14"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="8" t="s">
         <v>8</v>
       </c>
@@ -1141,21 +1153,21 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
-      <c r="H30"/>
+      <c r="H30" s="9"/>
       <c r="I30"/>
     </row>
     <row r="31" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="15"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="11"/>
-      <c r="H31"/>
+      <c r="H31" s="11"/>
       <c r="I31"/>
     </row>
     <row r="32" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1165,21 +1177,21 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="4"/>
-      <c r="H32"/>
+      <c r="H32" s="4"/>
       <c r="I32"/>
     </row>
     <row r="33" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B33" s="14"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="7"/>
-      <c r="H33"/>
+      <c r="H33" s="7"/>
       <c r="I33"/>
     </row>
     <row r="34" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B34" s="14"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="8" t="s">
         <v>36</v>
       </c>
@@ -1187,11 +1199,11 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="9"/>
-      <c r="H34"/>
+      <c r="H34" s="9"/>
       <c r="I34"/>
     </row>
     <row r="35" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="15"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="10" t="s">
         <v>37</v>
       </c>
@@ -1199,11 +1211,11 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="11"/>
-      <c r="H35"/>
+      <c r="H35" s="11"/>
       <c r="I35"/>
     </row>
     <row r="36" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1215,11 +1227,11 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="4"/>
-      <c r="H36"/>
+      <c r="H36" s="4"/>
       <c r="I36"/>
     </row>
     <row r="37" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B37" s="14"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="6" t="s">
         <v>40</v>
       </c>
@@ -1227,11 +1239,11 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="7"/>
-      <c r="H37"/>
+      <c r="H37" s="7"/>
       <c r="I37"/>
     </row>
     <row r="38" spans="2:9" ht="21" x14ac:dyDescent="0.3">
-      <c r="B38" s="14"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="8" t="s">
         <v>16</v>
       </c>
@@ -1241,11 +1253,11 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
-      <c r="H38"/>
+      <c r="H38" s="9"/>
       <c r="I38"/>
     </row>
     <row r="39" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="15"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="10" t="s">
         <v>41</v>
       </c>
@@ -1253,7 +1265,7 @@
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="11"/>
-      <c r="H39"/>
+      <c r="H39" s="11"/>
       <c r="I39"/>
     </row>
   </sheetData>
@@ -1269,6 +1281,6 @@
     <mergeCell ref="B12:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.25" top="0.94" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="94" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>